<commit_message>
[ais-704] refactored forming defects report
</commit_message>
<xml_diff>
--- a/files/defects/defects_pharmacy_template.xlsx
+++ b/files/defects/defects_pharmacy_template.xlsx
@@ -43,7 +43,7 @@
     <t>кол-во СКЮ входящих в АМ аптеки/магазина</t>
   </si>
   <si>
-    <t>кол-во СКЮ в дефектуре по АМ ЛС</t>
+    <t>кол-во СКЮ в дефектуре по АМ ПФ</t>
   </si>
   <si>
     <t>% дефектуры от АМ</t>
@@ -1117,17 +1117,23 @@
   <dimension ref="A1:N1505"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="35.875" customWidth="1"/>
-    <col min="2" max="2" width="30.328125" customWidth="1"/>
-    <col min="3" max="3" width="6.09375" customWidth="1"/>
+    <col min="2" max="2" width="46.609375" customWidth="1"/>
+    <col min="3" max="3" width="12.2421875" customWidth="1"/>
     <col min="4" max="4" width="13.8046875" customWidth="1"/>
+    <col min="6" max="6" width="18.2265625" customWidth="1"/>
+    <col min="7" max="7" width="10.2890625" customWidth="1"/>
+    <col min="9" max="9" width="17.3125" customWidth="1"/>
+    <col min="10" max="10" width="13.4140625" customWidth="1"/>
+    <col min="11" max="11" width="17.1875" customWidth="1"/>
     <col min="12" max="12" width="19.3984375" customWidth="1"/>
     <col min="13" max="13" width="29.296875" customWidth="1"/>
+    <col min="14" max="14" width="15.4921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">

</xml_diff>